<commit_message>
14.21 - Updated Test with Lego modules
</commit_message>
<xml_diff>
--- a/Accounting/Create Order/Default.xlsx
+++ b/Accounting/Create Order/Default.xlsx
@@ -19,12 +19,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+  <si>
+    <t>Order No</t>
+  </si>
+  <si>
+    <t>Denver</t>
+  </si>
+  <si>
+    <t>Samuel Mishler</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
   <si>
     <t>Order_Message</t>
   </si>
   <si>
+    <t>15-Jan-2020</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>FlyTo</t>
+  </si>
+  <si>
+    <t>Passenger</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>17-Jan-2021</t>
+  </si>
+  <si>
+    <t>Amir khan</t>
+  </si>
+  <si>
     <t>Order 141 completed</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Roger Wattenhofer</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>17-Jan-2023</t>
+  </si>
+  <si>
+    <t>Tickets</t>
+  </si>
+  <si>
+    <t>FlyFrom</t>
+  </si>
+  <si>
+    <t>Frankfurt</t>
   </si>
 </sst>
 </file>
@@ -169,12 +226,23 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -194,12 +262,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -498,24 +572,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="14.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.359375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.76171875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.41796875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.0625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.86328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
       <c t="s">
+        <v>4</v>
+      </c>
+      <c t="s">
         <v>0</v>
+      </c>
+      <c t="s">
+        <v>19</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="s">
+        <v>16</v>
+      </c>
+      <c t="s">
+        <v>3</v>
+      </c>
+      <c t="s">
+        <v>18</v>
+      </c>
+      <c t="s">
+        <v>8</v>
       </c>
     </row>
     <row>
-      <c s="2" t="s">
+      <c s="1" t="s">
+        <v>12</v>
+      </c>
+      <c s="1" t="str">
+        <f t="shared" si="0" ref="B2:B4">SUBSTITUTE(SUBSTITUTE(A2, "Order ", ""), " completed", "")</f>
+        <v>141</v>
+      </c>
+      <c s="1" t="s">
         <v>1</v>
+      </c>
+      <c s="1" t="s">
+        <v>20</v>
+      </c>
+      <c s="3" t="s">
+        <v>10</v>
+      </c>
+      <c s="1" t="s">
+        <v>13</v>
+      </c>
+      <c s="1">
+        <v>2</v>
+      </c>
+      <c s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="1" t="s">
+        <v>12</v>
+      </c>
+      <c s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>141</v>
+      </c>
+      <c s="1" t="s">
+        <v>9</v>
+      </c>
+      <c s="1" t="s">
+        <v>15</v>
+      </c>
+      <c s="3" t="s">
+        <v>5</v>
+      </c>
+      <c s="1" t="s">
+        <v>13</v>
+      </c>
+      <c s="1">
+        <v>2</v>
+      </c>
+      <c s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row>
+      <c s="1" t="s">
+        <v>12</v>
+      </c>
+      <c s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>141</v>
+      </c>
+      <c s="1" t="s">
+        <v>6</v>
+      </c>
+      <c s="1" t="s">
+        <v>15</v>
+      </c>
+      <c s="3" t="s">
+        <v>17</v>
+      </c>
+      <c s="1" t="s">
+        <v>13</v>
+      </c>
+      <c s="1">
+        <v>2</v>
+      </c>
+      <c s="4" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -533,7 +712,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>
@@ -547,12 +726,14 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="5" width="9.078125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.41796875" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>
@@ -571,7 +752,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>
@@ -590,7 +771,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>
@@ -609,7 +790,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>

</xml_diff>